<commit_message>
MAIN Adicionado o Estado KPI Connection para a introdução dos indicadores na Base de Dados
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,24 +5,34 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.t.pais\Documents\UiPath\DO_Diferimentos-Covid19\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.t.pais\Documents\UiPath\DO_Diferimentos-Covid19v2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2329AA-13EC-4E82-A211-EE23464788DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374C63D4-FF5C-4F3F-B174-74808B6D092E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="-24120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -152,13 +162,22 @@
   </si>
   <si>
     <t>Data\Input\Parametros.xlsx</t>
+  </si>
+  <si>
+    <t>URL Salesforce</t>
+  </si>
+  <si>
+    <t>https://credibom.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>Initial URL Salesforce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -189,6 +208,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,10 +232,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -223,8 +249,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,7 +568,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -651,7 +679,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1642,8 +1680,11 @@
     <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{633914B8-67CF-4227-80F3-05284514582C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>